<commit_message>
Updated data analysis spreadsheet to include YOLO results
</commit_message>
<xml_diff>
--- a/Data_analysis.xlsx
+++ b/Data_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blain\Documents\Git\TORCH_CLIP_FRCNN_Trainable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D523A30-6F58-42F3-91B3-599CE6C1FD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E076BA65-109F-4B41-B793-58144B16D0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{F3E7B00F-E8CD-4697-878A-A3ACE4518BB5}"/>
+    <workbookView xWindow="40050" yWindow="1650" windowWidth="28800" windowHeight="15225" activeTab="7" xr2:uid="{F3E7B00F-E8CD-4697-878A-A3ACE4518BB5}"/>
   </bookViews>
   <sheets>
     <sheet name="FRCNN .1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="CRPN No BCC .5" sheetId="4" r:id="rId4"/>
     <sheet name="CRPN BCC .1" sheetId="6" r:id="rId5"/>
     <sheet name="CRPN BCC .5" sheetId="7" r:id="rId6"/>
+    <sheet name="YOLO .1" sheetId="9" r:id="rId7"/>
+    <sheet name="YOLO .5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="33">
   <si>
     <t>clock</t>
   </si>
@@ -136,6 +138,9 @@
   </si>
   <si>
     <t>C-RPN - BCC eps = 35</t>
+  </si>
+  <si>
+    <t>YOLOv5</t>
   </si>
 </sst>
 </file>
@@ -2453,7 +2458,7 @@
         <v>0.6071428571428571</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" ref="C20:D20" si="0">AVERAGE(D5:D18)</f>
+        <f t="shared" ref="D20" si="0">AVERAGE(D5:D18)</f>
         <v>0.29928571428571427</v>
       </c>
       <c r="E20">
@@ -2558,7 +2563,7 @@
         <v>0.624</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" ref="C28:D28" si="1">AVERAGE(D22:D26)</f>
+        <f t="shared" ref="D28" si="1">AVERAGE(D22:D26)</f>
         <v>0.314</v>
       </c>
       <c r="E28">
@@ -2575,7 +2580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB7EECD-5CEE-4BA1-849A-23F90B83BC28}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5:F18"/>
     </sheetView>
   </sheetViews>
@@ -2868,7 +2873,7 @@
         <v>0.25142857142857145</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" ref="D20:E20" si="0">AVERAGE(D5:D18)</f>
+        <f t="shared" ref="D20" si="0">AVERAGE(D5:D18)</f>
         <v>0.12071428571428573</v>
       </c>
       <c r="E20">
@@ -2973,8 +2978,838 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" ref="D28:E28" si="1">AVERAGE(D22:D26)</f>
+        <f t="shared" ref="D28" si="1">AVERAGE(D22:D26)</f>
         <v>0.11000000000000001</v>
+      </c>
+      <c r="E28">
+        <v>417</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C688F5-0228-4E4E-92DD-EC8A622668D3}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:O25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.88</v>
+      </c>
+      <c r="C5">
+        <v>0.33</v>
+      </c>
+      <c r="D5">
+        <v>0.48</v>
+      </c>
+      <c r="E5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+      <c r="C6">
+        <v>0.67</v>
+      </c>
+      <c r="D6">
+        <v>0.64</v>
+      </c>
+      <c r="E6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.02</v>
+      </c>
+      <c r="D7">
+        <v>0.03</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.86</v>
+      </c>
+      <c r="C8">
+        <v>0.53</v>
+      </c>
+      <c r="D8">
+        <v>0.65</v>
+      </c>
+      <c r="E8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.79</v>
+      </c>
+      <c r="C9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D9">
+        <v>0.66</v>
+      </c>
+      <c r="E9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0.44</v>
+      </c>
+      <c r="C10">
+        <v>0.27</v>
+      </c>
+      <c r="D10">
+        <v>0.34</v>
+      </c>
+      <c r="E10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0.93</v>
+      </c>
+      <c r="C11">
+        <v>0.44</v>
+      </c>
+      <c r="D11">
+        <v>0.59</v>
+      </c>
+      <c r="E11">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0.78</v>
+      </c>
+      <c r="C12">
+        <v>0.94</v>
+      </c>
+      <c r="D12">
+        <v>0.86</v>
+      </c>
+      <c r="E12">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>0.92</v>
+      </c>
+      <c r="C13">
+        <v>0.78</v>
+      </c>
+      <c r="D13">
+        <v>0.85</v>
+      </c>
+      <c r="E13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0.75</v>
+      </c>
+      <c r="C14">
+        <v>0.77</v>
+      </c>
+      <c r="D14">
+        <v>0.76</v>
+      </c>
+      <c r="E14">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>0.82</v>
+      </c>
+      <c r="C15">
+        <v>0.72</v>
+      </c>
+      <c r="D15">
+        <v>0.77</v>
+      </c>
+      <c r="E15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>0.81</v>
+      </c>
+      <c r="C16">
+        <v>0.74</v>
+      </c>
+      <c r="D16">
+        <v>0.77</v>
+      </c>
+      <c r="E16">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>0.93</v>
+      </c>
+      <c r="C17">
+        <v>0.93</v>
+      </c>
+      <c r="D17">
+        <v>0.93</v>
+      </c>
+      <c r="E17">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>0.8</v>
+      </c>
+      <c r="C18">
+        <v>0.8</v>
+      </c>
+      <c r="D18">
+        <v>0.8</v>
+      </c>
+      <c r="E18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2">
+        <f>AVERAGE(B5:B18)</f>
+        <v>0.80785714285714294</v>
+      </c>
+      <c r="C20" s="2">
+        <f>AVERAGE(C5:C18)</f>
+        <v>0.60785714285714287</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" ref="D20" si="0">AVERAGE(D5:D18)</f>
+        <v>0.65214285714285702</v>
+      </c>
+      <c r="E20">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <f>AVERAGE(B22:B26)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <f>AVERAGE(C22:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" ref="D28" si="1">AVERAGE(D22:D26)</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>417</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A6A075-836F-499A-80E1-4FDD8349F8C0}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.71</v>
+      </c>
+      <c r="C5">
+        <v>0.27</v>
+      </c>
+      <c r="D5">
+        <v>0.39</v>
+      </c>
+      <c r="E5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C6">
+        <v>0.64</v>
+      </c>
+      <c r="D6">
+        <v>0.61</v>
+      </c>
+      <c r="E6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.02</v>
+      </c>
+      <c r="D7">
+        <v>0.03</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.83</v>
+      </c>
+      <c r="C8">
+        <v>0.51</v>
+      </c>
+      <c r="D8">
+        <v>0.63</v>
+      </c>
+      <c r="E8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.74</v>
+      </c>
+      <c r="C9">
+        <v>0.54</v>
+      </c>
+      <c r="D9">
+        <v>0.62</v>
+      </c>
+      <c r="E9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="C10">
+        <v>0.16</v>
+      </c>
+      <c r="D10">
+        <v>0.19</v>
+      </c>
+      <c r="E10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0.89</v>
+      </c>
+      <c r="C11">
+        <v>0.41</v>
+      </c>
+      <c r="D11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E11">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0.75</v>
+      </c>
+      <c r="C12">
+        <v>0.9</v>
+      </c>
+      <c r="D12">
+        <v>0.81</v>
+      </c>
+      <c r="E12">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+      <c r="C13">
+        <v>0.77</v>
+      </c>
+      <c r="D13">
+        <v>0.83</v>
+      </c>
+      <c r="E13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0.7</v>
+      </c>
+      <c r="C14">
+        <v>0.72</v>
+      </c>
+      <c r="D14">
+        <v>0.71</v>
+      </c>
+      <c r="E14">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>0.77</v>
+      </c>
+      <c r="C15">
+        <v>0.69</v>
+      </c>
+      <c r="D15">
+        <v>0.73</v>
+      </c>
+      <c r="E15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>0.61</v>
+      </c>
+      <c r="C16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D16">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E16">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>0.91</v>
+      </c>
+      <c r="C17">
+        <v>0.91</v>
+      </c>
+      <c r="D17">
+        <v>0.91</v>
+      </c>
+      <c r="E17">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>0.72</v>
+      </c>
+      <c r="C18">
+        <v>0.72</v>
+      </c>
+      <c r="D18">
+        <v>0.72</v>
+      </c>
+      <c r="E18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2">
+        <f>AVERAGE(B5:B18)</f>
+        <v>0.7400000000000001</v>
+      </c>
+      <c r="C20" s="2">
+        <f>AVERAGE(C5:C18)</f>
+        <v>0.55785714285714294</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" ref="D20" si="0">AVERAGE(D5:D18)</f>
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="E20">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <f>AVERAGE(B22:B26)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <f>AVERAGE(C22:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" ref="D28" si="1">AVERAGE(D22:D26)</f>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>417</v>

</xml_diff>